<commit_message>
Plots gemacht und Datentabelle erganzt
</commit_message>
<xml_diff>
--- a/Versuch8/datasets/gasthermometer.xlsx
+++ b/Versuch8/datasets/gasthermometer.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele Calvanese\Documents\Uni\Grundpraktikum\Grundpraktikum\Versuch8\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C14C961C-0E68-40FA-B627-BB38A4EB9FE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9115D2AF-2CFE-44F7-9BB8-C0EDB3AC9B53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14604" windowHeight="3672" activeTab="1" xr2:uid="{C1DF02A8-BD28-4226-AB01-C5E311576982}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="4392" activeTab="3" xr2:uid="{829F5D97-4205-46B8-A569-AB952F8C1C38}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="4392" xr2:uid="{829F5D97-4205-46B8-A569-AB952F8C1C38}"/>
   </bookViews>
   <sheets>
     <sheet name="Heat up" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="68">
   <si>
     <t>r1</t>
   </si>
@@ -223,7 +223,16 @@
     <t>vs: C9, C12</t>
   </si>
   <si>
-    <t>delta t</t>
+    <t>delta_t</t>
+  </si>
+  <si>
+    <t>delta_t_corr</t>
+  </si>
+  <si>
+    <t>delta_t_err</t>
+  </si>
+  <si>
+    <t>delta_t_corr_err</t>
   </si>
 </sst>
 </file>
@@ -582,13 +591,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED39F4AC-1D9D-4673-8BF0-E68A7CEC8386}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="1">
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -597,10 +606,14 @@
     <col min="12" max="12" width="11.6640625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="9.6640625" customWidth="1"/>
     <col min="14" max="14" width="13.21875" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+    <col min="15" max="15" width="8.88671875" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" customWidth="1"/>
+    <col min="19" max="19" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -646,8 +659,17 @@
       <c r="O1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -672,8 +694,8 @@
         <v>91575.940799999997</v>
       </c>
       <c r="H2">
-        <f>SQRT((F2*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F2*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I2">
         <f>(G2-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -681,7 +703,7 @@
       </c>
       <c r="J2">
         <f>SQRT((G2*$H$2)^2+($G$2*H2)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.56269052287646859</v>
+        <v>0.56806174011605959</v>
       </c>
       <c r="K2">
         <f>Constants!$D$2*(1+Constants!$E$8*I2)</f>
@@ -697,17 +719,29 @@
       </c>
       <c r="N2">
         <f>G2*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J2^2+(I2*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I2*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.9852228404642576E-2</v>
+        <v>2.0041729786159045E-2</v>
       </c>
       <c r="O2">
-        <f>M2-I2</f>
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
+        <f>I2-A2</f>
+        <v>-1</v>
+      </c>
+      <c r="P2">
+        <f>SQRT(J2^2+B2^2)</f>
+        <v>0.75676557835546776</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q12" si="0">M2-A2</f>
+        <v>-1</v>
+      </c>
+      <c r="R2">
+        <f>SQRT(N2^2+B2^2)</f>
+        <v>0.50040150972276387</v>
+      </c>
+      <c r="S2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10</v>
       </c>
@@ -735,8 +769,8 @@
         <v>95042.322367999994</v>
       </c>
       <c r="H3">
-        <f>SQRT((F3*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F3*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I3">
         <f>(G3-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -744,7 +778,7 @@
       </c>
       <c r="J3">
         <f>SQRT((G3*$H$2)^2+($G$2*H3)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.57343905284830687</v>
+        <v>0.5789128712285565</v>
       </c>
       <c r="K3">
         <f>Constants!$D$2*(1+Constants!$E$8*I3)</f>
@@ -760,29 +794,41 @@
       </c>
       <c r="N3">
         <f>G3*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J3^2+(I3*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I3*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.13591018899670673</v>
+        <v>0.13594129859675025</v>
       </c>
       <c r="O3">
-        <f>M3-I3</f>
-        <v>0.37859205508665283</v>
-      </c>
-      <c r="P3" t="s">
+        <f t="shared" ref="O3:O12" si="1">I3-A3</f>
+        <v>0.33942012528250487</v>
+      </c>
+      <c r="P3">
+        <f>SQRT(J3^2+B3^2)</f>
+        <v>0.76494451594484369</v>
+      </c>
+      <c r="Q3">
+        <f>M3-A3</f>
+        <v>0.7180121803691577</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R12" si="2">SQRT(N3^2+B3^2)</f>
+        <v>0.5181505926506027</v>
+      </c>
+      <c r="S3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20.5</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B12" si="0">B3</f>
+        <f t="shared" ref="B4:B12" si="3">B3</f>
         <v>0.5</v>
       </c>
       <c r="C4">
         <v>128</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D12" si="1">D3</f>
+        <f t="shared" ref="D4:D12" si="4">D3</f>
         <v>1</v>
       </c>
       <c r="E4">
@@ -790,7 +836,7 @@
         <v>28</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F12" si="2">F3</f>
+        <f t="shared" ref="F4:F12" si="5">F3</f>
         <v>1</v>
       </c>
       <c r="G4">
@@ -798,8 +844,8 @@
         <v>98642.026303999999</v>
       </c>
       <c r="H4">
-        <f>SQRT((F4*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F4*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I4">
         <f>(G4-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -807,7 +853,7 @@
       </c>
       <c r="J4">
         <f>SQRT((G4*$H$2)^2+($G$2*H4)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.58480246112788181</v>
+        <v>0.59038475002961777</v>
       </c>
       <c r="K4">
         <f>Constants!$D$2*(1+Constants!$E$8*I4)</f>
@@ -823,26 +869,38 @@
       </c>
       <c r="N4">
         <f>G4*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J4^2+(I4*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I4*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.28495651275031697</v>
+        <v>0.28497313686903158</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O12" si="3">M4-I4</f>
-        <v>0.80097500285694778</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>0.57651025538359235</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P12" si="6">SQRT(J4^2+B4^2)</f>
+        <v>0.77366281613344601</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q12" si="7">M4-A4</f>
+        <v>1.3774852582405401</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="2"/>
+        <v>0.57550820040810524</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>30.5</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C5">
         <v>151</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E5">
@@ -850,7 +908,7 @@
         <v>51</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G5">
@@ -858,8 +916,8 @@
         <v>101708.440768</v>
       </c>
       <c r="H5">
-        <f>SQRT((F5*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F5*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I5">
         <f>(G5-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -867,7 +925,7 @@
       </c>
       <c r="J5">
         <f>SQRT((G5*$H$2)^2+($G$2*H5)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.59463560741341559</v>
+        <v>0.6003117595715971</v>
       </c>
       <c r="K5">
         <f>Constants!$D$2*(1+Constants!$E$8*I5)</f>
@@ -883,26 +941,38 @@
       </c>
       <c r="N5">
         <f>G5*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J5^2+(I5*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I5*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.42068169535299593</v>
+        <v>0.42069407314969526</v>
       </c>
       <c r="O5">
-        <f t="shared" si="3"/>
-        <v>1.1842726423376853</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.27707963378956535</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>0.78126449342072823</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="7"/>
+        <v>0.90719300854811991</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="2"/>
+        <v>0.65343974717129139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>40.5</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C6">
         <v>174</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E6">
@@ -910,7 +980,7 @@
         <v>74</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G6">
@@ -918,8 +988,8 @@
         <v>104774.855232</v>
       </c>
       <c r="H6">
-        <f>SQRT((F6*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F6*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I6">
         <f>(G6-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -927,7 +997,7 @@
       </c>
       <c r="J6">
         <f>SQRT((G6*$H$2)^2+($G$2*H6)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.6046024319010963</v>
+        <v>0.61037372335403361</v>
       </c>
       <c r="K6">
         <f>Constants!$D$2*(1+Constants!$E$8*I6)</f>
@@ -943,26 +1013,38 @@
       </c>
       <c r="N6">
         <f>G6*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J6^2+(I6*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I6*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.56417629095345734</v>
+        <v>0.56418641659906765</v>
       </c>
       <c r="O6">
-        <f t="shared" si="3"/>
-        <v>1.5891810295918489</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-1.1306695229627266</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>0.78902223172802066</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="7"/>
+        <v>0.45851150662912232</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>0.75386093722575698</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>49.5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C7">
         <v>199</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E7">
@@ -970,7 +1052,7 @@
         <v>99</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G7">
@@ -978,8 +1060,8 @@
         <v>108107.91443200001</v>
       </c>
       <c r="H7">
-        <f>SQRT((F7*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F7*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I7">
         <f>(G7-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -987,7 +1069,7 @@
       </c>
       <c r="J7">
         <f>SQRT((G7*$H$2)^2+($G$2*H7)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.61557997642815354</v>
+        <v>0.62145605510251167</v>
       </c>
       <c r="K7">
         <f>Constants!$D$2*(1+Constants!$E$8*I7)</f>
@@ -1003,26 +1085,38 @@
       </c>
       <c r="N7">
         <f>G7*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J7^2+(I7*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I7*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.72889313027190006</v>
+        <v>0.72890178005161677</v>
       </c>
       <c r="O7">
-        <f t="shared" si="3"/>
-        <v>2.0538100869363873</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.18891940249876171</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>0.79762624607241706</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="7"/>
+        <v>1.8648906844376256</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="2"/>
+        <v>0.88391051863998971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>60</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C8">
         <v>226</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E8">
@@ -1030,7 +1124,7 @@
         <v>126</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G8">
@@ -1038,8 +1132,8 @@
         <v>111707.618368</v>
       </c>
       <c r="H8">
-        <f>SQRT((F8*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F8*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I8">
         <f>(G8-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1047,7 +1141,7 @@
       </c>
       <c r="J8">
         <f>SQRT((G8*$H$2)^2+($G$2*H8)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.62759540282899495</v>
+        <v>0.63358617592737743</v>
       </c>
       <c r="K8">
         <f>Constants!$D$2*(1+Constants!$E$8*I8)</f>
@@ -1063,26 +1157,38 @@
       </c>
       <c r="N8">
         <f>G8*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J8^2+(I8*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I8*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.91698885535612884</v>
+        <v>0.91699648574658577</v>
       </c>
       <c r="O8">
-        <f t="shared" si="3"/>
-        <v>2.5842876256491394</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>4.8170727602283137E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>0.80711302946134977</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>2.6324583532514225</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="2"/>
+        <v>1.0444532324961173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>70</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C9">
         <v>250</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E9">
@@ -1090,7 +1196,7 @@
         <v>150</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G9">
@@ -1098,8 +1204,8 @@
         <v>114907.35520000001</v>
       </c>
       <c r="H9">
-        <f>SQRT((F9*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F9*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I9">
         <f>(G9-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1107,7 +1213,7 @@
       </c>
       <c r="J9">
         <f>SQRT((G9*$H$2)^2+($G$2*H9)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.63840761475396701</v>
+        <v>0.64450159687529973</v>
       </c>
       <c r="K9">
         <f>Constants!$D$2*(1+Constants!$E$8*I9)</f>
@@ -1123,26 +1229,38 @@
       </c>
       <c r="N9">
         <f>G9*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J9^2+(I9*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I9*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.0930673816276875</v>
+        <v>1.0930743902229556</v>
       </c>
       <c r="O9">
-        <f t="shared" si="3"/>
-        <v>3.0808246856298638</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.4077491567522884</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>0.8157096961387742</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="7"/>
+        <v>2.6730755288775754</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="2"/>
+        <v>1.2020031707783829</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>80</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C10">
         <v>275</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E10">
@@ -1150,7 +1268,7 @@
         <v>175</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G10">
@@ -1158,8 +1276,8 @@
         <v>118240.41440000001</v>
       </c>
       <c r="H10">
-        <f>SQRT((F10*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F10*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I10">
         <f>(G10-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1167,7 +1285,7 @@
       </c>
       <c r="J10">
         <f>SQRT((G10*$H$2)^2+($G$2*H10)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.64979532567238341</v>
+        <v>0.65599801029841054</v>
       </c>
       <c r="K10">
         <f>Constants!$D$2*(1+Constants!$E$8*I10)</f>
@@ -1183,26 +1301,38 @@
       </c>
       <c r="N10">
         <f>G10*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J10^2+(I10*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I10*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.285366482230335</v>
+        <v>1.2853730202242244</v>
       </c>
       <c r="O10">
-        <f t="shared" si="3"/>
-        <v>3.6230726858280917</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <f>I10-A10</f>
+        <v>-0.46599903628832351</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="6"/>
+        <v>0.82482324743879132</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="7"/>
+        <v>3.1570736495397682</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>1.3791967956460545</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>90</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C11">
         <v>299</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E11">
@@ -1210,7 +1340,7 @@
         <v>199</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G11">
@@ -1218,8 +1348,8 @@
         <v>121440.151232</v>
       </c>
       <c r="H11">
-        <f>SQRT((F11*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F11*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I11">
         <f>(G11-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1227,7 +1357,7 @@
       </c>
       <c r="J11">
         <f>SQRT((G11*$H$2)^2+($G$2*H11)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.66084148107272289</v>
+        <v>0.66714960785195043</v>
       </c>
       <c r="K11">
         <f>Constants!$D$2*(1+Constants!$E$8*I11)</f>
@@ -1243,26 +1373,38 @@
       </c>
       <c r="N11">
         <f>G11*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J11^2+(I11*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I11*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.4784993620747495</v>
+        <v>1.4785055634023108</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
-        <v>4.1676517862276654</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.92191892064293768</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="6"/>
+        <v>0.83371973663636589</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="7"/>
+        <v>3.2457328655847277</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="2"/>
+        <v>1.5607622179600531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>97</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="C12">
         <v>317</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E12">
@@ -1270,7 +1412,7 @@
         <v>217</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="G12">
@@ -1278,8 +1420,8 @@
         <v>123839.95385600001</v>
       </c>
       <c r="H12">
-        <f>SQRT((F12*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F12*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I12">
         <f>(G12-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1287,7 +1429,7 @@
       </c>
       <c r="J12">
         <f>SQRT((G12*$H$2)^2+($G$2*H12)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.66919597988626855</v>
+        <v>0.67558385534835286</v>
       </c>
       <c r="K12">
         <f>Constants!$D$2*(1+Constants!$E$8*I12)</f>
@@ -1303,14 +1445,26 @@
       </c>
       <c r="N12">
         <f>G12*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J12^2+(I12*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I12*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.6288288010889809</v>
+        <v>1.6288348036903526</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
-        <v>4.5915281959477596</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="1"/>
+        <v>-0.76385883390888409</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>0.84048411383401178</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="7"/>
+        <v>3.8276693620388755</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="2"/>
+        <v>1.7038494116890111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1354,6 +1508,15 @@
         <v>10</v>
       </c>
       <c r="O13" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>10</v>
+      </c>
+      <c r="R13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1368,21 +1531,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0DF4D3F-2834-4CDB-AA8F-7D01B431A27E}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="11" max="12" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1428,8 +1596,17 @@
       <c r="O1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1454,8 +1631,8 @@
         <v>91575.940799999997</v>
       </c>
       <c r="H2">
-        <f>SQRT((F2*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F2*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I2">
         <f>(G2-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1463,7 +1640,7 @@
       </c>
       <c r="J2">
         <f>SQRT((G2*$H$2)^2+($G$2*H2)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.56269052287646859</v>
+        <v>0.56806174011605959</v>
       </c>
       <c r="K2">
         <f>Constants!$D$2*(1+Constants!$E$8*I2)</f>
@@ -1479,17 +1656,29 @@
       </c>
       <c r="N2">
         <f>G2*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J2^2+(I2*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I2*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.9852228404642576E-2</v>
+        <v>2.0041729786159045E-2</v>
       </c>
       <c r="O2">
-        <f>M2-I2</f>
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
+        <f t="shared" ref="O2:O11" si="0">I2-A2</f>
+        <v>-1</v>
+      </c>
+      <c r="P2">
+        <f>SQRT(J2^2+B2^2)</f>
+        <v>0.75676557835546776</v>
+      </c>
+      <c r="Q2">
+        <f>M2-A2</f>
+        <v>-1</v>
+      </c>
+      <c r="R2">
+        <f>SQRT(N2^2+B2^2)</f>
+        <v>0.50040150972276387</v>
+      </c>
+      <c r="S2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1517,8 +1706,8 @@
         <v>94242.388160000002</v>
       </c>
       <c r="H3">
-        <f>SQRT((F3*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F3*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I3">
         <f>(G3-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1526,7 +1715,7 @@
       </c>
       <c r="J3">
         <f>SQRT((G3*$H$2)^2+($G$2*H3)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.57094132088897243</v>
+        <v>0.57639129692531466</v>
       </c>
       <c r="K3">
         <f>Constants!$D$2*(1+Constants!$E$8*I3)</f>
@@ -1542,29 +1731,41 @@
       </c>
       <c r="N3">
         <f>G3*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J3^2+(I3*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I3*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.10449850631218775</v>
+        <v>0.10453794033030561</v>
       </c>
       <c r="O3">
-        <f>M3-I3</f>
-        <v>0.28877353324776589</v>
-      </c>
-      <c r="P3" t="s">
+        <f t="shared" si="0"/>
+        <v>-1.0465999036288194</v>
+      </c>
+      <c r="P3">
+        <f>SQRT(J3^2+B3^2)</f>
+        <v>0.76303795919419781</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q12" si="1">M3-A3</f>
+        <v>-0.75782637038105349</v>
+      </c>
+      <c r="R3">
+        <f>SQRT(N3^2+B3^2)</f>
+        <v>0.51081129682936977</v>
+      </c>
+      <c r="S3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B12" si="0">B3</f>
+        <f t="shared" ref="B4:B12" si="2">B3</f>
         <v>0.5</v>
       </c>
       <c r="C4">
         <v>125</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D12" si="1">D3</f>
+        <f t="shared" ref="D4:D12" si="3">D3</f>
         <v>1</v>
       </c>
       <c r="E4">
@@ -1572,7 +1773,7 @@
         <v>25</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F12" si="2">F3</f>
+        <f t="shared" ref="F4:F12" si="4">F3</f>
         <v>1</v>
       </c>
       <c r="G4">
@@ -1580,8 +1781,8 @@
         <v>98242.059200000003</v>
       </c>
       <c r="H4">
-        <f>SQRT((F4*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F4*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I4">
         <f>(G4-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1589,7 +1790,7 @@
       </c>
       <c r="J4">
         <f>SQRT((G4*$H$2)^2+($G$2*H4)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.58353008697578013</v>
+        <v>0.58910023030601077</v>
       </c>
       <c r="K4">
         <f>Constants!$D$2*(1+Constants!$E$8*I4)</f>
@@ -1605,26 +1806,38 @@
       </c>
       <c r="N4">
         <f>G4*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J4^2+(I4*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I4*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.26783352945399919</v>
+        <v>0.26785099691764641</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O12" si="3">M4-I4</f>
-        <v>0.7525728895089685</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-0.11649975907207022</v>
+      </c>
+      <c r="P4">
+        <f>SQRT(J4^2+B4^2)</f>
+        <v>0.7726830406748908</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>0.63607313043689828</v>
+      </c>
+      <c r="R4">
+        <f>SQRT(N4^2+B4^2)</f>
+        <v>0.56722496114837639</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>31</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C5">
         <v>150</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E5">
@@ -1632,7 +1845,7 @@
         <v>50</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G5">
@@ -1640,8 +1853,8 @@
         <v>101575.11840000001</v>
       </c>
       <c r="H5">
-        <f>SQRT((F5*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F5*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I5">
         <f>(G5-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1649,7 +1862,7 @@
       </c>
       <c r="J5">
         <f>SQRT((G5*$H$2)^2+($G$2*H5)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.59420525129737067</v>
+        <v>0.59987729544929347</v>
       </c>
       <c r="K5">
         <f>Constants!$D$2*(1+Constants!$E$8*I5)</f>
@@ -1665,26 +1878,38 @@
       </c>
       <c r="N5">
         <f>G5*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J5^2+(I5*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I5*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.41461835062755936</v>
+        <v>0.41463085840396358</v>
       </c>
       <c r="O5">
-        <f t="shared" si="3"/>
-        <v>1.1671581547506236</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-1.1747496386081053</v>
+      </c>
+      <c r="P5">
+        <f>SQRT(J5^2+B5^2)</f>
+        <v>0.78093070729454539</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>-7.5914838574817622E-3</v>
+      </c>
+      <c r="R5">
+        <f>SQRT(N5^2+B5^2)</f>
+        <v>0.64955272976164735</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>41</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C6">
         <v>177</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E6">
@@ -1692,7 +1917,7 @@
         <v>77</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G6">
@@ -1700,8 +1925,8 @@
         <v>105174.822336</v>
       </c>
       <c r="H6">
-        <f>SQRT((F6*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F6*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I6">
         <f>(G6-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1709,7 +1934,7 @@
       </c>
       <c r="J6">
         <f>SQRT((G6*$H$2)^2+($G$2*H6)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.60591196341597753</v>
+        <v>0.6116957551296488</v>
       </c>
       <c r="K6">
         <f>Constants!$D$2*(1+Constants!$E$8*I6)</f>
@@ -1725,26 +1950,38 @@
       </c>
       <c r="N6">
         <f>G6*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J6^2+(I6*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I6*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.58346207728851152</v>
+        <v>0.58347198592374916</v>
       </c>
       <c r="O6">
-        <f t="shared" si="3"/>
-        <v>1.6435883979920547</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-0.43765950850706048</v>
+      </c>
+      <c r="P6">
+        <f>SQRT(J6^2+B6^2)</f>
+        <v>0.79004537644595529</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>1.2059288894849942</v>
+      </c>
+      <c r="R6">
+        <f>SQRT(N6^2+B6^2)</f>
+        <v>0.76840064963390275</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>50</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C7">
         <v>199</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E7">
@@ -1752,7 +1989,7 @@
         <v>99</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G7">
@@ -1760,8 +1997,8 @@
         <v>108107.91443200001</v>
       </c>
       <c r="H7">
-        <f>SQRT((F7*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F7*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I7">
         <f>(G7-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1769,7 +2006,7 @@
       </c>
       <c r="J7">
         <f>SQRT((G7*$H$2)^2+($G$2*H7)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.61557997642815354</v>
+        <v>0.62145605510251167</v>
       </c>
       <c r="K7">
         <f>Constants!$D$2*(1+Constants!$E$8*I7)</f>
@@ -1785,26 +2022,38 @@
       </c>
       <c r="N7">
         <f>G7*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J7^2+(I7*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I7*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.72889313027190006</v>
+        <v>0.72890178005161677</v>
       </c>
       <c r="O7">
-        <f t="shared" si="3"/>
-        <v>2.0538100869363873</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-0.68891940249876171</v>
+      </c>
+      <c r="P7">
+        <f>SQRT(J7^2+B7^2)</f>
+        <v>0.79762624607241706</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>1.3648906844376256</v>
+      </c>
+      <c r="R7">
+        <f>SQRT(N7^2+B7^2)</f>
+        <v>0.88391051863998971</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>59.5</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C8">
         <v>222</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E8">
@@ -1812,7 +2061,7 @@
         <v>122</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G8">
@@ -1820,8 +2069,8 @@
         <v>111174.32889600001</v>
       </c>
       <c r="H8">
-        <f>SQRT((F8*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F8*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I8">
         <f>(G8-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1829,7 +2078,7 @@
       </c>
       <c r="J8">
         <f>SQRT((G8*$H$2)^2+($G$2*H8)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.62580523222856621</v>
+        <v>0.63177891707896883</v>
       </c>
       <c r="K8">
         <f>Constants!$D$2*(1+Constants!$E$8*I8)</f>
@@ -1845,26 +2094,38 @@
       </c>
       <c r="N8">
         <f>G8*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J8^2+(I8*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I8*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>0.88845498490334751</v>
+        <v>0.88846274090016752</v>
       </c>
       <c r="O8">
-        <f t="shared" si="3"/>
-        <v>2.5038191651961341</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-1.0425092916719194</v>
+      </c>
+      <c r="P8">
+        <f>SQRT(J8^2+B8^2)</f>
+        <v>0.80569510366234354</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>1.4613098735242147</v>
+      </c>
+      <c r="R8">
+        <f>SQRT(N8^2+B8^2)</f>
+        <v>1.0194930318387851</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>70</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C9">
         <v>250</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E9">
@@ -1872,7 +2133,7 @@
         <v>150</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G9">
@@ -1880,8 +2141,8 @@
         <v>114907.35520000001</v>
       </c>
       <c r="H9">
-        <f>SQRT((F9*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F9*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I9">
         <f>(G9-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1889,7 +2150,7 @@
       </c>
       <c r="J9">
         <f>SQRT((G9*$H$2)^2+($G$2*H9)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.63840761475396701</v>
+        <v>0.64450159687529973</v>
       </c>
       <c r="K9">
         <f>Constants!$D$2*(1+Constants!$E$8*I9)</f>
@@ -1905,26 +2166,38 @@
       </c>
       <c r="N9">
         <f>G9*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J9^2+(I9*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I9*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.0930673816276875</v>
+        <v>1.0930743902229556</v>
       </c>
       <c r="O9">
-        <f t="shared" si="3"/>
-        <v>3.0808246856298638</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-0.4077491567522884</v>
+      </c>
+      <c r="P9">
+        <f>SQRT(J9^2+B9^2)</f>
+        <v>0.8157096961387742</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>2.6730755288775754</v>
+      </c>
+      <c r="R9">
+        <f>SQRT(N9^2+B9^2)</f>
+        <v>1.2020031707783829</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>79</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C10">
         <v>277</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E10">
@@ -1932,7 +2205,7 @@
         <v>177</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G10">
@@ -1940,8 +2213,8 @@
         <v>118507.059136</v>
       </c>
       <c r="H10">
-        <f>SQRT((F10*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F10*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I10">
         <f>(G10-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -1949,7 +2222,7 @@
       </c>
       <c r="J10">
         <f>SQRT((G10*$H$2)^2+($G$2*H10)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.65071165609777526</v>
+        <v>0.65692308764520591</v>
       </c>
       <c r="K10">
         <f>Constants!$D$2*(1+Constants!$E$8*I10)</f>
@@ -1965,26 +2238,38 @@
       </c>
       <c r="N10">
         <f>G10*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J10^2+(I10*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I10*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.3011419281541368</v>
+        <v>1.3011484343538495</v>
       </c>
       <c r="O10">
-        <f t="shared" si="3"/>
-        <v>3.6675555318739015</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1.3293409733487493</v>
+      </c>
+      <c r="P10">
+        <f>SQRT(J10^2+B10^2)</f>
+        <v>0.82555916994562595</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="1"/>
+        <v>4.9968965052226508</v>
+      </c>
+      <c r="R10">
+        <f>SQRT(N10^2+B10^2)</f>
+        <v>1.3939107748423045</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>89</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C11">
         <v>298</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E11">
@@ -1992,7 +2277,7 @@
         <v>198</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G11">
@@ -2000,8 +2285,8 @@
         <v>121306.82886400001</v>
       </c>
       <c r="H11">
-        <f>SQRT((F11*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F11*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I11">
         <f>(G11-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -2009,7 +2294,7 @@
       </c>
       <c r="J11">
         <f>SQRT((G11*$H$2)^2+($G$2*H11)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.66037907028055065</v>
+        <v>0.66668278307248374</v>
       </c>
       <c r="K11">
         <f>Constants!$D$2*(1+Constants!$E$8*I11)</f>
@@ -2025,26 +2310,38 @@
       </c>
       <c r="N11">
         <f>G11*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J11^2+(I11*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I11*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.4702854387413331</v>
+        <v>1.4702916523237102</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
-        <v>4.1444911915130263</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>-0.31958892546148832</v>
+      </c>
+      <c r="P11">
+        <f>SQRT(J11^2+B11^2)</f>
+        <v>0.83334622651408963</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="1"/>
+        <v>3.8249022660515379</v>
+      </c>
+      <c r="R11">
+        <f>SQRT(N11^2+B11^2)</f>
+        <v>1.5529834329099541</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>97</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="C12">
         <v>317</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="E12">
@@ -2052,7 +2349,7 @@
         <v>217</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="G12">
@@ -2060,8 +2357,8 @@
         <v>123839.95385600001</v>
       </c>
       <c r="H12">
-        <f>SQRT((F12*Constants!$B$8)^2 + Constants!$B$4)</f>
-        <v>133.3935366092654</v>
+        <f>SQRT((F12*Constants!$B$8)^2 + Constants!$B$4^2)</f>
+        <v>134.66685761674037</v>
       </c>
       <c r="I12">
         <f>(G12-$G$2)/(Constants!$C$8*$G$2)</f>
@@ -2069,7 +2366,7 @@
       </c>
       <c r="J12">
         <f>SQRT((G12*$H$2)^2+($G$2*H12)^2)/(Constants!$C$8*$G$2^2)</f>
-        <v>0.66919597988626855</v>
+        <v>0.67558385534835286</v>
       </c>
       <c r="K12">
         <f>Constants!$D$2*(1+Constants!$E$8*I12)</f>
@@ -2085,14 +2382,26 @@
       </c>
       <c r="N12">
         <f>G12*Constants!$D$8/$G$2*SQRT((Constants!$E$8+Vols!$C$9/(Constants!$F$10*Vols!$A$9))^2*J12^2+(I12*Vols!$C$12/(Constants!$F$10*Vols!$A$9))^2+(I12*Vols!$C$9*Vols!$C$12/(Constants!$F$10*Vols!$A$9^2))^2)</f>
-        <v>1.6288288010889809</v>
+        <v>1.6288348036903526</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="O12" si="5">M12-I12</f>
         <v>4.5915281959477596</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P12">
+        <f>SQRT(J12^2+B12^2)</f>
+        <v>0.84048411383401178</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="1"/>
+        <v>3.8276693620388755</v>
+      </c>
+      <c r="R12">
+        <f>SQRT(N12^2+B12^2)</f>
+        <v>1.7038494116890111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2136,6 +2445,15 @@
         <v>10</v>
       </c>
       <c r="O13" t="s">
+        <v>10</v>
+      </c>
+      <c r="P13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>10</v>
+      </c>
+      <c r="R13" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2152,7 +2470,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
     <sheetView zoomScaleNormal="100" workbookViewId="1">
       <selection activeCell="B4" sqref="B4"/>
@@ -2292,9 +2610,9 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="1">
+    <sheetView topLeftCell="A2" workbookViewId="1">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Kleine Korrektur in der Datentabelle
</commit_message>
<xml_diff>
--- a/Versuch8/datasets/gasthermometer.xlsx
+++ b/Versuch8/datasets/gasthermometer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michele Calvanese\Documents\Uni\Grundpraktikum\Grundpraktikum\Versuch8\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9115D2AF-2CFE-44F7-9BB8-C0EDB3AC9B53}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AA6CD35-441C-4ADC-AD0D-16BD201376E7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14604" windowHeight="3672" activeTab="1" xr2:uid="{C1DF02A8-BD28-4226-AB01-C5E311576982}"/>
     <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="4392" xr2:uid="{829F5D97-4205-46B8-A569-AB952F8C1C38}"/>
@@ -597,7 +597,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="1">
-      <selection activeCell="P5" sqref="P5"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,7 +730,7 @@
         <v>0.75676557835546776</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q12" si="0">M2-A2</f>
+        <f t="shared" ref="Q2" si="0">M2-A2</f>
         <v>-1</v>
       </c>
       <c r="R2">
@@ -1534,7 +1534,7 @@
   <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="N1" sqref="N1"/>
@@ -1659,11 +1659,11 @@
         <v>2.0041729786159045E-2</v>
       </c>
       <c r="O2">
-        <f t="shared" ref="O2:O11" si="0">I2-A2</f>
+        <f t="shared" ref="O2:O12" si="0">I2-A2</f>
         <v>-1</v>
       </c>
       <c r="P2">
-        <f>SQRT(J2^2+B2^2)</f>
+        <f t="shared" ref="P2:P12" si="1">SQRT(J2^2+B2^2)</f>
         <v>0.75676557835546776</v>
       </c>
       <c r="Q2">
@@ -1671,7 +1671,7 @@
         <v>-1</v>
       </c>
       <c r="R2">
-        <f>SQRT(N2^2+B2^2)</f>
+        <f t="shared" ref="R2:R12" si="2">SQRT(N2^2+B2^2)</f>
         <v>0.50040150972276387</v>
       </c>
       <c r="S2" t="s">
@@ -1738,15 +1738,15 @@
         <v>-1.0465999036288194</v>
       </c>
       <c r="P3">
-        <f>SQRT(J3^2+B3^2)</f>
+        <f t="shared" si="1"/>
         <v>0.76303795919419781</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q12" si="1">M3-A3</f>
+        <f t="shared" ref="Q3:Q12" si="3">M3-A3</f>
         <v>-0.75782637038105349</v>
       </c>
       <c r="R3">
-        <f>SQRT(N3^2+B3^2)</f>
+        <f t="shared" si="2"/>
         <v>0.51081129682936977</v>
       </c>
       <c r="S3" t="s">
@@ -1758,14 +1758,14 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B12" si="2">B3</f>
+        <f t="shared" ref="B4:B12" si="4">B3</f>
         <v>0.5</v>
       </c>
       <c r="C4">
         <v>125</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D12" si="3">D3</f>
+        <f t="shared" ref="D4:D12" si="5">D3</f>
         <v>1</v>
       </c>
       <c r="E4">
@@ -1773,7 +1773,7 @@
         <v>25</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F12" si="4">F3</f>
+        <f t="shared" ref="F4:F12" si="6">F3</f>
         <v>1</v>
       </c>
       <c r="G4">
@@ -1813,15 +1813,15 @@
         <v>-0.11649975907207022</v>
       </c>
       <c r="P4">
-        <f>SQRT(J4^2+B4^2)</f>
+        <f t="shared" si="1"/>
         <v>0.7726830406748908</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.63607313043689828</v>
       </c>
       <c r="R4">
-        <f>SQRT(N4^2+B4^2)</f>
+        <f t="shared" si="2"/>
         <v>0.56722496114837639</v>
       </c>
     </row>
@@ -1830,14 +1830,14 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C5">
         <v>150</v>
       </c>
       <c r="D5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E5">
@@ -1845,7 +1845,7 @@
         <v>50</v>
       </c>
       <c r="F5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G5">
@@ -1885,15 +1885,15 @@
         <v>-1.1747496386081053</v>
       </c>
       <c r="P5">
-        <f>SQRT(J5^2+B5^2)</f>
+        <f t="shared" si="1"/>
         <v>0.78093070729454539</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>-7.5914838574817622E-3</v>
       </c>
       <c r="R5">
-        <f>SQRT(N5^2+B5^2)</f>
+        <f t="shared" si="2"/>
         <v>0.64955272976164735</v>
       </c>
     </row>
@@ -1902,14 +1902,14 @@
         <v>41</v>
       </c>
       <c r="B6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C6">
         <v>177</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E6">
@@ -1917,7 +1917,7 @@
         <v>77</v>
       </c>
       <c r="F6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G6">
@@ -1957,15 +1957,15 @@
         <v>-0.43765950850706048</v>
       </c>
       <c r="P6">
-        <f>SQRT(J6^2+B6^2)</f>
+        <f t="shared" si="1"/>
         <v>0.79004537644595529</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.2059288894849942</v>
       </c>
       <c r="R6">
-        <f>SQRT(N6^2+B6^2)</f>
+        <f t="shared" si="2"/>
         <v>0.76840064963390275</v>
       </c>
     </row>
@@ -1974,14 +1974,14 @@
         <v>50</v>
       </c>
       <c r="B7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C7">
         <v>199</v>
       </c>
       <c r="D7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E7">
@@ -1989,7 +1989,7 @@
         <v>99</v>
       </c>
       <c r="F7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G7">
@@ -2029,15 +2029,15 @@
         <v>-0.68891940249876171</v>
       </c>
       <c r="P7">
-        <f>SQRT(J7^2+B7^2)</f>
+        <f t="shared" si="1"/>
         <v>0.79762624607241706</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.3648906844376256</v>
       </c>
       <c r="R7">
-        <f>SQRT(N7^2+B7^2)</f>
+        <f t="shared" si="2"/>
         <v>0.88391051863998971</v>
       </c>
     </row>
@@ -2046,14 +2046,14 @@
         <v>59.5</v>
       </c>
       <c r="B8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C8">
         <v>222</v>
       </c>
       <c r="D8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E8">
@@ -2061,7 +2061,7 @@
         <v>122</v>
       </c>
       <c r="F8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G8">
@@ -2101,15 +2101,15 @@
         <v>-1.0425092916719194</v>
       </c>
       <c r="P8">
-        <f>SQRT(J8^2+B8^2)</f>
+        <f t="shared" si="1"/>
         <v>0.80569510366234354</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.4613098735242147</v>
       </c>
       <c r="R8">
-        <f>SQRT(N8^2+B8^2)</f>
+        <f t="shared" si="2"/>
         <v>1.0194930318387851</v>
       </c>
     </row>
@@ -2118,14 +2118,14 @@
         <v>70</v>
       </c>
       <c r="B9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C9">
         <v>250</v>
       </c>
       <c r="D9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E9">
@@ -2133,7 +2133,7 @@
         <v>150</v>
       </c>
       <c r="F9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G9">
@@ -2173,15 +2173,15 @@
         <v>-0.4077491567522884</v>
       </c>
       <c r="P9">
-        <f>SQRT(J9^2+B9^2)</f>
+        <f t="shared" si="1"/>
         <v>0.8157096961387742</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.6730755288775754</v>
       </c>
       <c r="R9">
-        <f>SQRT(N9^2+B9^2)</f>
+        <f t="shared" si="2"/>
         <v>1.2020031707783829</v>
       </c>
     </row>
@@ -2190,14 +2190,14 @@
         <v>79</v>
       </c>
       <c r="B10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C10">
         <v>277</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E10">
@@ -2205,7 +2205,7 @@
         <v>177</v>
       </c>
       <c r="F10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G10">
@@ -2245,15 +2245,15 @@
         <v>1.3293409733487493</v>
       </c>
       <c r="P10">
-        <f>SQRT(J10^2+B10^2)</f>
+        <f t="shared" si="1"/>
         <v>0.82555916994562595</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.9968965052226508</v>
       </c>
       <c r="R10">
-        <f>SQRT(N10^2+B10^2)</f>
+        <f t="shared" si="2"/>
         <v>1.3939107748423045</v>
       </c>
     </row>
@@ -2262,14 +2262,14 @@
         <v>89</v>
       </c>
       <c r="B11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C11">
         <v>298</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E11">
@@ -2277,7 +2277,7 @@
         <v>198</v>
       </c>
       <c r="F11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G11">
@@ -2317,15 +2317,15 @@
         <v>-0.31958892546148832</v>
       </c>
       <c r="P11">
-        <f>SQRT(J11^2+B11^2)</f>
+        <f t="shared" si="1"/>
         <v>0.83334622651408963</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.8249022660515379</v>
       </c>
       <c r="R11">
-        <f>SQRT(N11^2+B11^2)</f>
+        <f t="shared" si="2"/>
         <v>1.5529834329099541</v>
       </c>
     </row>
@@ -2334,14 +2334,14 @@
         <v>97</v>
       </c>
       <c r="B12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="C12">
         <v>317</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="E12">
@@ -2349,7 +2349,7 @@
         <v>217</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G12">
@@ -2385,19 +2385,19 @@
         <v>1.6288348036903526</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12" si="5">M12-I12</f>
-        <v>4.5915281959477596</v>
+        <f t="shared" si="0"/>
+        <v>-0.76385883390888409</v>
       </c>
       <c r="P12">
-        <f>SQRT(J12^2+B12^2)</f>
+        <f t="shared" si="1"/>
         <v>0.84048411383401178</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.8276693620388755</v>
       </c>
       <c r="R12">
-        <f>SQRT(N12^2+B12^2)</f>
+        <f t="shared" si="2"/>
         <v>1.7038494116890111</v>
       </c>
     </row>

</xml_diff>